<commit_message>
Commiting the changes made in revC -Some documents related to revC design have also be included -some datasheets still missing
</commit_message>
<xml_diff>
--- a/PCBs/Projects/MotorController/CAM/BOM_reformatted.xlsx
+++ b/PCBs/Projects/MotorController/CAM/BOM_reformatted.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1585,8 +1585,8 @@
   </sheetPr>
   <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4107,6 +4107,6 @@
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToWidth="2" orientation="portrait" r:id="rId60"/>
+  <pageSetup scale="47" fitToHeight="0" orientation="landscape" r:id="rId60"/>
 </worksheet>
 </file>
</xml_diff>